<commit_message>
completed experiments and wrote report
Report compares simulation and real quantum computing
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="4650" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -345,7 +345,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,6 +498,9 @@
       <c r="A19">
         <v>20</v>
       </c>
+      <c r="B19">
+        <v>46810.004110336296</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>